<commit_message>
Handle missing cell values for both XSSF and HSSF excel handlers
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/cars93.xlsx
+++ b/src/test/resources/xls/cars93.xlsx
@@ -1612,7 +1612,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>

</xml_diff>